<commit_message>
Ligera optimización del Random Forest
</commit_message>
<xml_diff>
--- a/AB-Analytics-R/datasets/cpi/CPI-Archive-2012-2023.xlsx
+++ b/AB-Analytics-R/datasets/cpi/CPI-Archive-2012-2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubi6\Escritorio\Universidad\Analytics\AB analytics\AB--ADVANCED-PROGRAMMING-FOR-DATA-ANALYSIS--1\AB-Analytics-R\datasets\cpi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDA1206-3C2F-4205-9F43-0DE9DAE9EBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C05D869-7E4F-45CB-A91D-BF4FC72A5843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1152,10 +1152,10 @@
     <t>PRI</t>
   </si>
   <si>
-    <t>ISO</t>
+    <t>score</t>
   </si>
   <si>
-    <t>score</t>
+    <t>iso</t>
   </si>
 </sst>
 </file>
@@ -2511,7 +2511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15.75"/>
@@ -2529,7 +2529,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>370</v>
@@ -2538,7 +2538,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="11" customFormat="1" ht="15">
@@ -38797,18 +38797,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -38950,18 +38950,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80F9B26F-C52B-4546-AAB3-2BD3CCE827B6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3FD084C-1DF1-406C-B7AB-5B65D825AF2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3FD084C-1DF1-406C-B7AB-5B65D825AF2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80F9B26F-C52B-4546-AAB3-2BD3CCE827B6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>